<commit_message>
Training on full corpora, one file and one value of n (3 to 6) at a time. Twitter is done already.
</commit_message>
<xml_diff>
--- a/buy the book.xlsx
+++ b/buy the book.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmitrytoda\Documents\R\SwiftPredict\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8961141-DC42-465A-B3D0-6DF4271B481C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1219958D-532A-4DF9-AD9A-2D02B55DCDF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{B296383C-4F09-4712-AA01-F4AB8D3E5D2B}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <definedName name="alpha">Sheet1!$A$16</definedName>
     <definedName name="alpha_sellthe">Sheet1!$A$19</definedName>
     <definedName name="alpha_the">Sheet1!$A$16</definedName>
+    <definedName name="alphaBT1">Sheet1!$A$22</definedName>
     <definedName name="disc">Sheet1!$A$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="49">
   <si>
     <t>unigram</t>
   </si>
@@ -179,6 +180,15 @@
   </si>
   <si>
     <t>alpha(sell the)</t>
+  </si>
+  <si>
+    <t>alpha(book the)</t>
+  </si>
+  <si>
+    <t>alpha=1</t>
+  </si>
+  <si>
+    <t>2-gram</t>
   </si>
 </sst>
 </file>
@@ -202,12 +212,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -222,12 +250,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,17 +576,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584E5254-1073-462C-A58E-44300B72123A}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -600,8 +634,8 @@
         <v>5</v>
       </c>
       <c r="F2">
-        <f>E2-disc</f>
-        <v>4.5</v>
+        <f t="shared" ref="F2:F8" si="0">E2-disc</f>
+        <v>4.3</v>
       </c>
       <c r="H2" t="s">
         <v>18</v>
@@ -610,8 +644,8 @@
         <v>4</v>
       </c>
       <c r="J2">
-        <f>I2-disc</f>
-        <v>3.5</v>
+        <f t="shared" ref="J2:J7" si="1">I2-disc</f>
+        <v>3.3</v>
       </c>
       <c r="L2" t="s">
         <v>30</v>
@@ -631,8 +665,8 @@
         <v>6</v>
       </c>
       <c r="F3">
-        <f>E3-disc</f>
-        <v>5.5</v>
+        <f t="shared" si="0"/>
+        <v>5.3</v>
       </c>
       <c r="H3" t="s">
         <v>19</v>
@@ -641,18 +675,18 @@
         <v>2</v>
       </c>
       <c r="J3">
-        <f>I3-disc</f>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>1.3</v>
       </c>
       <c r="L3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>6</v>
       </c>
       <c r="D4" t="s">
@@ -662,8 +696,8 @@
         <v>3</v>
       </c>
       <c r="F4">
-        <f>E4-disc</f>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H4" t="s">
         <v>20</v>
@@ -672,18 +706,18 @@
         <v>1</v>
       </c>
       <c r="J4">
-        <f>I4-disc</f>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
         <v>8</v>
       </c>
       <c r="D5" t="s">
@@ -693,8 +727,8 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <f>E5-disc</f>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>21</v>
@@ -703,18 +737,18 @@
         <v>1</v>
       </c>
       <c r="J5">
-        <f>I5-disc</f>
-        <v>0.5</v>
+        <f t="shared" si="1"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -724,8 +758,8 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <f>E6-disc</f>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
       </c>
       <c r="H6" t="s">
         <v>22</v>
@@ -734,18 +768,18 @@
         <v>5</v>
       </c>
       <c r="J6">
-        <f>I6-disc</f>
-        <v>4.5</v>
+        <f t="shared" si="1"/>
+        <v>4.3</v>
       </c>
       <c r="L6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -755,8 +789,8 @@
         <v>5</v>
       </c>
       <c r="F7" s="1">
-        <f>E7-disc</f>
-        <v>4.5</v>
+        <f t="shared" si="0"/>
+        <v>4.3</v>
       </c>
       <c r="H7" t="s">
         <v>23</v>
@@ -765,18 +799,18 @@
         <v>3</v>
       </c>
       <c r="J7">
-        <f>I7-disc</f>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="6">
         <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -786,8 +820,8 @@
         <v>3</v>
       </c>
       <c r="F8" s="1">
-        <f>E8-disc</f>
-        <v>2.5</v>
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L8" t="s">
         <v>33</v>
@@ -815,7 +849,7 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -825,7 +859,7 @@
       </c>
       <c r="E13">
         <f>F7/SUM(E7:E8)</f>
-        <v>0.5625</v>
+        <v>0.53749999999999998</v>
       </c>
       <c r="G13" t="str">
         <f>_xlfn.CONCAT("sell the ",A2)</f>
@@ -836,22 +870,22 @@
       </c>
       <c r="I13">
         <f>J5/E6</f>
-        <v>0.5</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E14">
         <f>F8/SUM(E7:E8)</f>
-        <v>0.3125</v>
-      </c>
-      <c r="G14" t="str">
-        <f t="shared" ref="G14:G19" si="0">_xlfn.CONCAT("sell the ",A3)</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="G14" s="4" t="str">
+        <f t="shared" ref="G14:G19" si="2">_xlfn.CONCAT("sell the ",A3)</f>
         <v>sell the house</v>
       </c>
       <c r="H14" t="s">
@@ -859,7 +893,7 @@
       </c>
       <c r="I14">
         <f>alpha_sellthe*E14/SUM(E$14:E$19)</f>
-        <v>0.35714285714285715</v>
+        <v>0.43513513513513508</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -869,134 +903,248 @@
       <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D15" s="6" t="str">
         <f>_xlfn.CONCAT("the ", A4)</f>
         <v>the buy</v>
       </c>
       <c r="E15">
         <f>alpha_the*B4/SUM(B$4:B$8)</f>
-        <v>3.125E-2</v>
+        <v>4.3750000000000011E-2</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sell the buy</v>
       </c>
       <c r="H15" t="s">
         <v>44</v>
       </c>
       <c r="I15">
-        <f>alpha_sellthe*E15/SUM(E$14:E$19)</f>
-        <v>3.5714285714285712E-2</v>
+        <f t="shared" ref="I15:I19" si="3">alpha_sellthe*E15/SUM(E$14:E$19)</f>
+        <v>6.6216216216216234E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>1-SUM(E13:E14)</f>
-        <v>0.125</v>
+        <v>0.17500000000000004</v>
       </c>
       <c r="C16" t="s">
         <v>39</v>
       </c>
-      <c r="D16" t="str">
+      <c r="D16" s="6" t="str">
         <f>_xlfn.CONCAT("the ", A5)</f>
         <v>the EOS</v>
       </c>
       <c r="E16">
         <f>alpha_the*B5/SUM(B$4:B$8)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>5.8333333333333348E-2</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sell the EOS</v>
       </c>
       <c r="H16" t="s">
         <v>44</v>
       </c>
       <c r="I16">
-        <f>alpha_sellthe*E16/SUM(E$14:E$19)</f>
-        <v>4.7619047619047616E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>8.8288288288288302E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>39</v>
       </c>
-      <c r="D17" t="str">
+      <c r="D17" s="6" t="str">
         <f>_xlfn.CONCAT("the ", A6)</f>
         <v>the paint</v>
       </c>
       <c r="E17">
         <f>alpha_the*B6/SUM(B$4:B$8)</f>
-        <v>5.208333333333333E-3</v>
+        <v>7.2916666666666685E-3</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sell the paint</v>
       </c>
       <c r="H17" t="s">
         <v>44</v>
       </c>
       <c r="I17">
-        <f>alpha_sellthe*E17/SUM(E$14:E$19)</f>
-        <v>5.9523809523809521E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1.1036036036036038E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>45</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="str">
+      <c r="D18" s="6" t="str">
         <f>_xlfn.CONCAT("the ", A7)</f>
         <v>the sell</v>
       </c>
       <c r="E18">
         <f>alpha_the*B7/SUM(B$4:B$8)</f>
-        <v>5.208333333333333E-3</v>
+        <v>7.2916666666666685E-3</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sell the sell</v>
       </c>
       <c r="H18" t="s">
         <v>44</v>
       </c>
       <c r="I18">
-        <f>alpha_sellthe*E18/SUM(E$14:E$19)</f>
-        <v>5.9523809523809521E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <f t="shared" si="3"/>
+        <v>1.1036036036036038E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <f>1-SUM(I13)</f>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="C19" t="s">
         <v>39</v>
       </c>
-      <c r="D19" t="str">
+      <c r="D19" s="6" t="str">
         <f>_xlfn.CONCAT("the ", A8)</f>
         <v>the the</v>
       </c>
       <c r="E19">
         <f>alpha_the*B8/SUM(B$4:B$8)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>5.8333333333333348E-2</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sell the the</v>
       </c>
       <c r="H19" t="s">
         <v>44</v>
       </c>
       <c r="I19">
-        <f>alpha_sellthe*E19/SUM(E$14:E$19)</f>
-        <v>4.7619047619047616E-2</v>
+        <f t="shared" si="3"/>
+        <v>8.8288288288288302E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>46</v>
+      </c>
+      <c r="I21" t="s">
+        <v>47</v>
+      </c>
+      <c r="J21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="str">
+        <f>_xlfn.CONCAT("book the ",A2)</f>
+        <v>book the book</v>
+      </c>
+      <c r="H22" t="s">
+        <v>44</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ref="I22:I28" si="4">alphaBT1*E13/SUM(E$13:E$19)</f>
+        <v>0.53749999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G23" t="str">
+        <f t="shared" ref="G23:G28" si="5">_xlfn.CONCAT("book the ",A3)</f>
+        <v>book the house</v>
+      </c>
+      <c r="H23" t="s">
+        <v>44</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="4"/>
+        <v>0.28749999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G24" t="str">
+        <f t="shared" si="5"/>
+        <v>book the buy</v>
+      </c>
+      <c r="H24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="4"/>
+        <v>4.3750000000000011E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G25" t="str">
+        <f t="shared" si="5"/>
+        <v>book the EOS</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="4"/>
+        <v>5.8333333333333348E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G26" t="str">
+        <f t="shared" si="5"/>
+        <v>book the paint</v>
+      </c>
+      <c r="H26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="4"/>
+        <v>7.2916666666666685E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G27" t="str">
+        <f t="shared" si="5"/>
+        <v>book the sell</v>
+      </c>
+      <c r="H27" t="s">
+        <v>44</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="4"/>
+        <v>7.2916666666666685E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G28" t="str">
+        <f t="shared" si="5"/>
+        <v>book the the</v>
+      </c>
+      <c r="H28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="4"/>
+        <v>5.8333333333333348E-2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J20:K20"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1044,15 +1192,15 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f>C2/SUM(C$2:C$8)</f>
+        <f t="shared" ref="D2:D8" si="0">C2/SUM(C$2:C$8)</f>
         <v>1</v>
       </c>
       <c r="E2">
-        <f>C2+1</f>
+        <f t="shared" ref="E2:E8" si="1">C2+1</f>
         <v>2</v>
       </c>
       <c r="F2">
-        <f>E2/SUM(E$2:E$8)</f>
+        <f t="shared" ref="F2:F8" si="2">E2/SUM(E$2:E$8)</f>
         <v>0.25</v>
       </c>
       <c r="G2">
@@ -1060,7 +1208,7 @@
         <v>1</v>
       </c>
       <c r="H2">
-        <f>G2/SUM(G$2:G$8)</f>
+        <f t="shared" ref="H2:H8" si="3">G2/SUM(G$2:G$8)</f>
         <v>0.49999999999999989</v>
       </c>
     </row>
@@ -1076,23 +1224,23 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <f>C3/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E3">
-        <f>C3+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F3">
-        <f>E3/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G3">
-        <f>(C3+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" ref="G3:G8" si="4">(C3+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="H3">
-        <f>G3/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
@@ -1108,23 +1256,23 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <f>C4/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E4">
-        <f>C4+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f>E4/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G4">
-        <f>(C4+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H4">
-        <f>G4/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
@@ -1140,23 +1288,23 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <f>C5/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>C5+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F5">
-        <f>E5/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G5">
-        <f>(C5+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H5">
-        <f>G5/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
@@ -1172,23 +1320,23 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <f>C6/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E6">
-        <f>C6+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F6">
-        <f>E6/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G6">
-        <f>(C6+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H6">
-        <f>G6/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
@@ -1204,23 +1352,23 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <f>C7/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E7">
-        <f>C7+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F7">
-        <f>E7/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G7">
-        <f>(C7+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H7">
-        <f>G7/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>
@@ -1236,23 +1384,23 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <f>C8/SUM(C$2:C$8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E8">
-        <f>C8+1</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F8">
-        <f>E8/SUM(E$2:E$8)</f>
+        <f t="shared" si="2"/>
         <v>0.125</v>
       </c>
       <c r="G8">
-        <f>(C8+1)*COUNT(C$2)/COUNT(C$3:C$8)</f>
+        <f t="shared" si="4"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="H8">
-        <f>G8/SUM(G$2:G$8)</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333315E-2</v>
       </c>
     </row>

</xml_diff>